<commit_message>
Edit Task&Progresses - API&Front
</commit_message>
<xml_diff>
--- a/docs/dataX_project_specification.xlsx
+++ b/docs/dataX_project_specification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/highsoul/dataX/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37070D3-3E98-DD42-B695-1476CF153282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB42910-A71B-B843-9B32-8F0264DDAECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9300" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9320" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="モデル設計_テーブル" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="399">
   <si>
     <t>No</t>
   </si>
@@ -932,9 +932,6 @@
     <t>ダッシュボード</t>
   </si>
   <si>
-    <t>Rakeバッチ処理連動</t>
-  </si>
-  <si>
     <t>ワークスペース脱退</t>
   </si>
   <si>
@@ -953,18 +950,6 @@
     <t>クエリパラメータで処理</t>
   </si>
   <si>
-    <t>エラー応答フォメット</t>
-  </si>
-  <si>
-    <t>エラーが発生する際の返信フォーマット</t>
-  </si>
-  <si>
-    <t>共通</t>
-  </si>
-  <si>
-    <t>全API共通仕様、後述別定義</t>
-  </si>
-  <si>
     <t>pending'</t>
   </si>
   <si>
@@ -1356,6 +1341,12 @@
   </si>
   <si>
     <t>helper methodで使用</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Rakeバッチ処理連動、cronの環境設定ができなかったため、bashファイルで迂回</t>
   </si>
 </sst>
 </file>
@@ -1941,10 +1932,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>133</v>
@@ -1961,8 +1952,8 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2084,7 +2075,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>135</v>
@@ -2098,7 +2089,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>30</v>
@@ -2458,7 +2449,7 @@
         <v>69</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>95</v>
@@ -2689,7 +2680,7 @@
     </row>
     <row r="36" spans="1:9" s="20" customFormat="1">
       <c r="A36" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>67</v>
@@ -2712,7 +2703,7 @@
     </row>
     <row r="37" spans="1:9" s="20" customFormat="1">
       <c r="A37" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>75</v>
@@ -2729,7 +2720,7 @@
     </row>
     <row r="38" spans="1:9" s="20" customFormat="1">
       <c r="A38" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>104</v>
@@ -2749,7 +2740,7 @@
     </row>
     <row r="39" spans="1:9" s="20" customFormat="1">
       <c r="A39" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>92</v>
@@ -2772,7 +2763,7 @@
     </row>
     <row r="40" spans="1:9" s="20" customFormat="1">
       <c r="A40" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>79</v>
@@ -2789,7 +2780,7 @@
     </row>
     <row r="41" spans="1:9" s="20" customFormat="1">
       <c r="A41" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>81</v>
@@ -3290,11 +3281,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3306,7 +3297,7 @@
     <col min="5" max="5" width="34.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
@@ -3331,13 +3322,13 @@
         <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3423,16 +3414,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>186</v>
@@ -3542,7 +3533,7 @@
         <v>186</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>137</v>
@@ -3559,7 +3550,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>224</v>
@@ -3588,13 +3579,13 @@
         <v>222</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>137</v>
@@ -3605,7 +3596,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>183</v>
@@ -3614,13 +3605,13 @@
         <v>222</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>137</v>
@@ -3631,22 +3622,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>175</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>137</v>
@@ -3672,7 +3663,7 @@
         <v>186</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>137</v>
@@ -3689,7 +3680,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>230</v>
@@ -3698,7 +3689,7 @@
         <v>186</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>137</v>
@@ -3709,16 +3700,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>186</v>
@@ -3750,7 +3741,7 @@
         <v>186</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>137</v>
@@ -3776,7 +3767,7 @@
         <v>186</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>137</v>
@@ -3787,7 +3778,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>35</v>
@@ -3796,13 +3787,13 @@
         <v>240</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>137</v>
@@ -3828,7 +3819,7 @@
         <v>186</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>137</v>
@@ -3854,7 +3845,7 @@
         <v>186</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>137</v>
@@ -3880,7 +3871,7 @@
         <v>186</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="18" customFormat="1">
@@ -3903,10 +3894,10 @@
         <v>186</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3914,22 +3905,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3943,7 +3937,7 @@
         <v>175</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>250</v>
@@ -3952,7 +3946,10 @@
         <v>186</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3966,7 +3963,7 @@
         <v>180</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>252</v>
@@ -3975,7 +3972,10 @@
         <v>186</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3998,7 +3998,10 @@
         <v>186</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4006,13 +4009,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>233</v>
@@ -4021,7 +4024,10 @@
         <v>186</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>373</v>
+        <v>368</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -4029,7 +4035,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>175</v>
@@ -4038,13 +4044,16 @@
         <v>232</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -4052,22 +4061,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -4075,22 +4087,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -4098,7 +4113,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>35</v>
@@ -4116,59 +4131,39 @@
         <v>259</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>398</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>186</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="2">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4237,7 +4232,7 @@
         <v>174</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>201</v>
@@ -4283,7 +4278,7 @@
         <v>174</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>201</v>
@@ -4329,7 +4324,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>201</v>
@@ -4375,7 +4370,7 @@
         <v>182</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>201</v>
@@ -4398,7 +4393,7 @@
         <v>184</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>201</v>
@@ -4421,7 +4416,7 @@
         <v>184</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>201</v>
@@ -4438,7 +4433,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>184</v>
@@ -4461,13 +4456,13 @@
         <v>18</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>217</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>201</v>
@@ -4475,16 +4470,16 @@
     </row>
     <row r="13" spans="1:7" ht="16">
       <c r="A13" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>217</v>
@@ -4496,7 +4491,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="11" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>30</v>
@@ -4511,7 +4506,7 @@
         <v>226</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>201</v>
@@ -4519,7 +4514,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="11" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>30</v>
@@ -4528,13 +4523,13 @@
         <v>18</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>231</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>201</v>
@@ -4551,10 +4546,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>153</v>
@@ -4565,22 +4560,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="11" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>201</v>
@@ -4597,10 +4592,10 @@
         <v>18</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>153</v>
@@ -4611,19 +4606,19 @@
     </row>
     <row r="19" spans="1:7" ht="16">
       <c r="A19" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="11" t="s">
@@ -4632,19 +4627,19 @@
     </row>
     <row r="20" spans="1:7" ht="16">
       <c r="A20" s="11" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>150</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="11" t="s">
@@ -4653,22 +4648,22 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="11" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>201</v>
@@ -4685,13 +4680,13 @@
         <v>18</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>201</v>
@@ -4708,13 +4703,13 @@
         <v>18</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>249</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>201</v>
@@ -4722,23 +4717,23 @@
     </row>
     <row r="24" spans="1:7" ht="16">
       <c r="A24" s="11" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="11" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4749,61 +4744,61 @@
         <v>30</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>169</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16">
       <c r="A26" s="11" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="11" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16">
       <c r="A27" s="11" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="11" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4860,7 +4855,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>11</v>
@@ -4869,7 +4864,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4883,7 +4878,7 @@
         <v>203</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>204</v>
@@ -4903,13 +4898,13 @@
         <v>189</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>204</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4923,13 +4918,13 @@
         <v>12</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>204</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -4941,7 +4936,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>179</v>
@@ -4950,7 +4945,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4961,7 +4956,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>208</v>
@@ -4970,24 +4965,24 @@
         <v>21</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F8" s="14">
         <v>3</v>
@@ -4995,59 +4990,59 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="14" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="14" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>225</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F11" s="14">
         <v>5</v>
@@ -5055,59 +5050,59 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="14" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="13" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F14" s="14">
         <v>21</v>
@@ -5115,59 +5110,59 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="14" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="14" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="14" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>150</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F17" s="17">
         <v>45809</v>
@@ -5175,47 +5170,47 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="14" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="14" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="14" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>135</v>
@@ -5227,7 +5222,7 @@
         <v>256</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F20" s="14">
         <v>1</v>
@@ -5235,19 +5230,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>256</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F21" s="14">
         <v>7</v>
@@ -5255,19 +5250,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="14" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>256</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F22" s="14">
         <v>10</v>
@@ -5275,19 +5270,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="14" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>256</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F23" s="14">
         <v>70</v>

</xml_diff>

<commit_message>
Edit document & Final commit
</commit_message>
<xml_diff>
--- a/docs/dataX_project_specification.xlsx
+++ b/docs/dataX_project_specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/highsoul/dataX/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49D061B-3356-7547-BBA7-9E474904BB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660C80A8-7A7D-F347-98E6-62A0C538F8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9320" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="572">
   <si>
     <t>No</t>
   </si>
@@ -1570,9 +1570,6 @@
     <t>複数担当者</t>
   </si>
   <si>
-    <t>自動的なSystem ruby使用でbash script活用、crontabに直接設定</t>
-  </si>
-  <si>
     <t>テスク対象</t>
   </si>
   <si>
@@ -1856,6 +1853,38 @@
   </si>
   <si>
     <t>進行率集計</t>
+  </si>
+  <si>
+    <t>・開発期間</t>
+  </si>
+  <si>
+    <t>05/12（月）から05/19(月）までです。</t>
+  </si>
+  <si>
+    <t>・開発環境</t>
+  </si>
+  <si>
+    <t>・MacBook Pro(M1 Pro)
+・macOS Sequoia 15.5
+・Visual Studio Code
+・Postman</t>
+  </si>
+  <si>
+    <t>・開発言語</t>
+  </si>
+  <si>
+    <t>・Ruby on Rails(Back)
+・SQLite3(DB)
+・Vue + Vite + Pug(Front)</t>
+  </si>
+  <si>
+    <t>ユニットテスト実行</t>
+  </si>
+  <si>
+    <t>自動的なSystem ruby使用でbash script活用、crontabを直接設定</t>
+  </si>
+  <si>
+    <t>Team-Task-Manager</t>
   </si>
 </sst>
 </file>
@@ -1987,7 +2016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2011,29 +2040,49 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2339,167 +2388,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA16080-D4E5-484F-BFA8-E106F093FC0D}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="258" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B7" activeCellId="1" sqref="B2 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="45.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="23" t="s">
+      <c r="A2" s="20" t="s">
+        <v>571</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="15" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="32">
-      <c r="A4" s="16" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:4" ht="32">
+      <c r="A5" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="17" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="20" t="s">
+        <v>563</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>564</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4" ht="64">
+      <c r="A7" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="48">
+      <c r="A8" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>568</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="29" t="s">
         <v>393</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="18" t="s">
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="30" t="s">
         <v>394</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>391</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="21" t="s">
-        <v>499</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="21" t="s">
-        <v>500</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="21" t="s">
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="28" t="s">
         <v>385</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="22" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="22" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="31" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="21" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="28" t="s">
         <v>388</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="22" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="31" t="s">
         <v>389</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="21" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>569</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" location="モデル設計_テーブル!A1" display="モデル設計（テーブル）" xr:uid="{B0F8E34F-650B-FA4F-A94E-73D4EC225DF9}"/>
-    <hyperlink ref="A10" location="モデル設計_カラム!A1" display="モデル設計（カラム）" xr:uid="{36D45B54-B613-1F46-B731-2ABCADE5CD60}"/>
-    <hyperlink ref="A11" location="機能設計_API概要!A1" display="機能設計（API概要）" xr:uid="{9806E231-3639-5F49-A6AE-8B8D0CFEC0A7}"/>
-    <hyperlink ref="A12" location="機能設計_パラメータ!A1" display="機能設計（パラメータ）" xr:uid="{5BA8FAE0-1239-2B4F-84F3-A61F433C79CB}"/>
-    <hyperlink ref="A13" location="機能設計_戻り値!A1" display="機能設計（戻りキー）" xr:uid="{11439847-9E24-C041-8217-8A52031DB851}"/>
-    <hyperlink ref="A14" location="画面仕様書!A1" display="画面仕様書" xr:uid="{CCA9C9A2-7C23-9D41-935D-4971CB18EF69}"/>
-    <hyperlink ref="A15" location="Rake処理設計!A1" display="Rake処理設計" xr:uid="{82899257-A43F-BA4D-8303-DA45F57193B0}"/>
-    <hyperlink ref="A16" location="テストケース一覧!A1" display="テストケース一覧" xr:uid="{916DC701-ACD0-9C49-969A-277401923918}"/>
+    <hyperlink ref="A11" location="モデル設計_テーブル!A1" display="モデル設計（テーブル）" xr:uid="{B0F8E34F-650B-FA4F-A94E-73D4EC225DF9}"/>
+    <hyperlink ref="A12" location="モデル設計_カラム!A1" display="モデル設計（カラム）" xr:uid="{36D45B54-B613-1F46-B731-2ABCADE5CD60}"/>
+    <hyperlink ref="A13" location="機能設計_API概要!A1" display="機能設計（API概要）" xr:uid="{9806E231-3639-5F49-A6AE-8B8D0CFEC0A7}"/>
+    <hyperlink ref="A14" location="機能設計_パラメータ!A1" display="機能設計（パラメータ）" xr:uid="{5BA8FAE0-1239-2B4F-84F3-A61F433C79CB}"/>
+    <hyperlink ref="A15" location="機能設計_戻り値!A1" display="機能設計（戻りキー）" xr:uid="{11439847-9E24-C041-8217-8A52031DB851}"/>
+    <hyperlink ref="A16" location="画面仕様書!A1" display="画面仕様書" xr:uid="{CCA9C9A2-7C23-9D41-935D-4971CB18EF69}"/>
+    <hyperlink ref="A17" location="Rake処理設計!A1" display="Rake処理設計" xr:uid="{82899257-A43F-BA4D-8303-DA45F57193B0}"/>
+    <hyperlink ref="A18" location="テストケース一覧!A1" display="テストケース一覧" xr:uid="{916DC701-ACD0-9C49-969A-277401923918}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2523,7 +2600,6 @@
     <col min="5" max="5" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="2"/>
-    <col min="8" max="8" width="28" style="28"/>
     <col min="9" max="16384" width="28" style="2"/>
   </cols>
   <sheetData>
@@ -2568,7 +2644,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="15" t="s">
         <v>192</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -2578,7 +2654,7 @@
         <v>193</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>194</v>
@@ -2598,12 +2674,12 @@
         <v>179</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="16" t="s">
         <v>317</v>
       </c>
     </row>
@@ -2618,15 +2694,15 @@
         <v>10</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
@@ -2659,7 +2735,7 @@
         <v>276</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>15</v>
@@ -2669,7 +2745,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="15" t="s">
         <v>277</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -2679,7 +2755,7 @@
         <v>311</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>278</v>
@@ -2699,7 +2775,7 @@
         <v>249</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>278</v>
@@ -2719,7 +2795,7 @@
         <v>281</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>278</v>
@@ -2729,7 +2805,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="15" t="s">
         <v>283</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -2739,7 +2815,7 @@
         <v>267</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>284</v>
@@ -2759,7 +2835,7 @@
         <v>256</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>284</v>
@@ -2779,17 +2855,17 @@
         <v>313</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>284</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="15" t="s">
         <v>288</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -2799,7 +2875,7 @@
         <v>314</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>289</v>
@@ -2819,7 +2895,7 @@
         <v>259</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>289</v>
@@ -2839,7 +2915,7 @@
         <v>263</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>289</v>
@@ -2859,12 +2935,12 @@
         <v>295</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="17">
         <v>45809</v>
       </c>
     </row>
@@ -2879,7 +2955,7 @@
         <v>297</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>289</v>
@@ -2899,7 +2975,7 @@
         <v>315</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>289</v>
@@ -2919,7 +2995,7 @@
         <v>193</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>302</v>
@@ -2939,7 +3015,7 @@
         <v>304</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>302</v>
@@ -2959,7 +3035,7 @@
         <v>306</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>302</v>
@@ -2979,7 +3055,7 @@
         <v>316</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>302</v>
@@ -3029,7 +3105,7 @@
       <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -7685,26 +7761,26 @@
     <col min="8" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="27" customFormat="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:7" s="18" customFormat="1">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="18" t="s">
+        <v>468</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>469</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="18" t="s">
         <v>471</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="18" t="s">
         <v>472</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>473</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -7713,19 +7789,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7733,19 +7809,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>516</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7753,19 +7829,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>522</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="7" customFormat="1">
@@ -7773,19 +7849,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>524</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="7" customFormat="1">
@@ -7793,19 +7869,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>516</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="7" customFormat="1">
@@ -7813,19 +7889,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>481</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7833,19 +7909,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7853,19 +7929,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>478</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -7873,19 +7949,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>481</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7893,19 +7969,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>483</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -7913,19 +7989,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="7" customFormat="1">
@@ -7933,19 +8009,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>489</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1">
@@ -7953,19 +8029,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>493</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="7" customFormat="1">
@@ -7973,19 +8049,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>477</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>495</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="7" customFormat="1">
@@ -7993,19 +8069,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>498</v>
-      </c>
       <c r="F16" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -8013,19 +8089,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -8033,19 +8109,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>516</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -8053,19 +8129,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>481</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1">
@@ -8073,19 +8149,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>505</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="7" customFormat="1">
@@ -8093,19 +8169,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>478</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1">
@@ -8113,19 +8189,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>481</v>
-      </c>
       <c r="F22" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1">
@@ -8133,19 +8209,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>510</v>
-      </c>
       <c r="F23" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -8153,19 +8229,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -8173,19 +8249,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -8245,7 +8321,6 @@
     <col min="6" max="6" width="34.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="2"/>
-    <col min="9" max="9" width="31" style="28"/>
     <col min="10" max="16384" width="31" style="2"/>
   </cols>
   <sheetData>
@@ -8381,7 +8456,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>191</v>
@@ -8424,7 +8499,7 @@
         <v>179</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>270</v>
@@ -8570,7 +8645,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="13" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>24</v>
@@ -8579,10 +8654,10 @@
         <v>13</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>542</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>543</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>255</v>
@@ -8605,7 +8680,7 @@
         <v>256</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>144</v>
@@ -8628,7 +8703,7 @@
         <v>266</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>258</v>
@@ -8651,7 +8726,7 @@
         <v>259</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>144</v>
@@ -8674,7 +8749,7 @@
         <v>260</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>191</v>
@@ -8694,7 +8769,7 @@
         <v>262</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>191</v>
@@ -8702,7 +8777,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>127</v>
@@ -8714,10 +8789,10 @@
         <v>267</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>191</v>
@@ -8734,10 +8809,10 @@
         <v>13</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>548</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>549</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>255</v>
@@ -8771,7 +8846,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="13" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>127</v>
@@ -8780,13 +8855,13 @@
         <v>252</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>244</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -8809,12 +8884,12 @@
         <v>160</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>127</v>
@@ -8829,12 +8904,12 @@
         <v>244</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>24</v>
@@ -8843,13 +8918,13 @@
         <v>252</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>244</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>